<commit_message>
Eliminando múltiplas sentenças para o mesmo processo + Analisando se é dano ambiental
</commit_message>
<xml_diff>
--- a/docs/sentencas_acessaveis.xlsx
+++ b/docs/sentencas_acessaveis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C393"/>
+  <dimension ref="A1:D393"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>Download copia</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Publicado em</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -462,6 +467,11 @@
           <t>http://jud-anexos.digesto.com.br/0cacd6d80c499ae25dcb85380a07c3dd.pdf</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2021-08-13</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -475,6 +485,11 @@
           <t>http://jud-anexos.digesto.com.br/90df1f9ac9917f6df4b9f91915b3a8bd.pdf</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2022-05-16</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -488,6 +503,11 @@
           <t>http://jud-anexos.digesto.com.br/c89c7a26febccd44703bb340de170f09.pdf</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2022-07-20</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -501,6 +521,11 @@
           <t>http://jud-anexos.digesto.com.br/585fdfebfdd6d2ded0146d6b79813e2f.pdf</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2024-07-31</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -514,6 +539,11 @@
           <t>http://jud-anexos.digesto.com.br/6be7e9beac86d76d02b031e258dd81f3.pdf</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-01-29</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -527,6 +557,11 @@
           <t>http://jud-anexos.digesto.com.br/209b98634c9c4a3f7c83d1c521c5b8d6.pdf</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2022-09-14</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -540,6 +575,11 @@
           <t>http://jud-anexos.digesto.com.br/9e6f89021ad2692964ba32eda8dbf752.html</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-01-10</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -553,6 +593,11 @@
           <t>http://jud-anexos.digesto.com.br/d6ecb52b7493cb254b3188065a7134be.html</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2024-10-09</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -566,6 +611,11 @@
           <t>http://jud-anexos.digesto.com.br/ae7e8fe9bd0ffaae6c5a50b0550ad270.html</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2024-10-16</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -579,6 +629,11 @@
           <t>http://jud-anexos.digesto.com.br/2e196251a32e640f42b5b1fae06c7329.html</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-03-03</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -592,6 +647,11 @@
           <t>http://jud-anexos.digesto.com.br/a00473a504122143575a731b7c39ca8c.html</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2024-12-18</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -605,6 +665,11 @@
           <t>http://jud-anexos.digesto.com.br/95b9349b12d1987412f17a791acc906a.html</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-01-07</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -618,6 +683,11 @@
           <t>http://jud-anexos.digesto.com.br/7cef4bd654c356d84d7a617351f802cc.pdf</t>
         </is>
       </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2018-08-27</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -631,6 +701,11 @@
           <t>http://jud-anexos.digesto.com.br/1c8e3d1ddaf02c96f790919dedcc2c98.html</t>
         </is>
       </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2018-08-27</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -644,6 +719,11 @@
           <t>http://jud-anexos.digesto.com.br/d5d876cd4f1b1b52385f1ec4df9886ba.html</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2022-06-08</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -657,6 +737,11 @@
           <t>http://jud-anexos.digesto.com.br/3c06d880622cb6b027242835177f7a1c.html</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2022-08-16</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -670,6 +755,11 @@
           <t>http://jud-anexos.digesto.com.br/24586eb78e174455c03d488d6518e16c.html</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2020-07-06</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -683,6 +773,11 @@
           <t>http://jud-anexos.digesto.com.br/be70db0dae0a1d1f18eb65dfd5523e76.html</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-03-07</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -696,6 +791,11 @@
           <t>http://jud-anexos.digesto.com.br/806b3bed99f6b144980640e291ea43f5.html</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2024-12-18</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -709,6 +809,11 @@
           <t>http://jud-anexos.digesto.com.br/7cce4fed8abf878e5603e6b0f5562673.html</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2024-09-05</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -722,6 +827,11 @@
           <t>http://jud-anexos.digesto.com.br/81ecf2169bea0a34068e17cd743b84df.html</t>
         </is>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2024-10-14</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -735,6 +845,11 @@
           <t>http://jud-anexos.digesto.com.br/4d9968d3a030fe7f959689bec23ac635.html</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2024-11-11</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -748,6 +863,11 @@
           <t>http://jud-anexos.digesto.com.br/1cdff09e1ed2c127e91f31e5a5d223ac.html</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2025-02-06</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -761,6 +881,11 @@
           <t>http://jud-anexos.digesto.com.br/5631abc57e085f5121b0ead2d78e9e85.html</t>
         </is>
       </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2024-04-30</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -774,6 +899,11 @@
           <t>http://jud-anexos.digesto.com.br/25afbf7fded56e9b963e05b9f2b6bb1b.pdf</t>
         </is>
       </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>2023-12-12</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -787,6 +917,11 @@
           <t>http://jud-anexos.digesto.com.br/af2e31ab1171eebaf9eaba7298a863f1.pdf</t>
         </is>
       </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>2024-06-03</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -800,6 +935,11 @@
           <t>http://jud-anexos.digesto.com.br/39dff1c665a4058e993ad23403b74d3f.pdf</t>
         </is>
       </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -813,6 +953,11 @@
           <t>http://jud-anexos.digesto.com.br/baa70e5f7e80b87ec2513996dc999998.pdf</t>
         </is>
       </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>2024-11-08</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -826,6 +971,11 @@
           <t>http://jud-anexos.digesto.com.br/b66f11432ff40098fd8950223d3646fe.pdf</t>
         </is>
       </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>2024-11-08</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -839,6 +989,11 @@
           <t>http://jud-anexos.digesto.com.br/c1189054a28c83134ddf407f0fdffbee.pdf</t>
         </is>
       </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>2024-01-26</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -852,6 +1007,11 @@
           <t>http://jud-anexos.digesto.com.br/205d76f4d06f3a2aa127976ad1c9d6c8.pdf</t>
         </is>
       </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>2021-10-12</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -865,6 +1025,11 @@
           <t>http://jud-anexos.digesto.com.br/a322a1e63179ad2a721b9268801dbfb6.pdf</t>
         </is>
       </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>2020-04-06</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -878,6 +1043,11 @@
           <t>http://jud-anexos.digesto.com.br/09d6be65c301338f50831f289070bf32.pdf</t>
         </is>
       </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>2021-08-09</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -891,6 +1061,11 @@
           <t>http://jud-anexos.digesto.com.br/b168533f3d6d3898c82f4dd6eb1244fc.html</t>
         </is>
       </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2021-08-09</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -904,6 +1079,11 @@
           <t>http://jud-anexos.digesto.com.br/907b9608e50b4c2ae6f6bd6e2937e8c1.pdf</t>
         </is>
       </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2024-07-20</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -917,6 +1097,11 @@
           <t>http://jud-anexos.digesto.com.br/805e361e1816efe094ff01def94456b1.pdf</t>
         </is>
       </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -930,6 +1115,11 @@
           <t>http://jud-anexos.digesto.com.br/300db9de92c641853aa4fccd85039f66.html</t>
         </is>
       </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -943,6 +1133,11 @@
           <t>http://jud-anexos.digesto.com.br/f8941539197bdd583e3bdd448abb2e6c.html</t>
         </is>
       </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2024-03-18</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -956,6 +1151,11 @@
           <t>http://jud-anexos.digesto.com.br/c7fac8749343a02deddd5dfdcb5092e1.html</t>
         </is>
       </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -969,6 +1169,11 @@
           <t>http://jud-anexos.digesto.com.br/39ff161134b9cf8983c1fbdb72a6399a.html</t>
         </is>
       </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2024-05-30</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -982,6 +1187,11 @@
           <t>http://jud-anexos.digesto.com.br/5d0a8e5ed8f0a7fec125a2c66852472a.html</t>
         </is>
       </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2024-07-18</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -995,6 +1205,11 @@
           <t>http://jud-anexos.digesto.com.br/4da50e667aeda4f63db0ec57a8ed181c.html</t>
         </is>
       </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2024-06-19</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1008,6 +1223,11 @@
           <t>http://jud-anexos.digesto.com.br/62974e3deafad97342e0730ae6127cc0.html</t>
         </is>
       </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2022-10-07</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1021,6 +1241,11 @@
           <t>http://jud-anexos.digesto.com.br/a19aa35b716dceaa7412de65748a8282.html</t>
         </is>
       </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2024-09-12</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1034,6 +1259,11 @@
           <t>http://jud-anexos.digesto.com.br/d29b30e83ac5c3c14263ead70dff3ab3.html</t>
         </is>
       </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2024-06-28</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -1047,6 +1277,11 @@
           <t>http://jud-anexos.digesto.com.br/aa49f40feb6ffc4d1d587640b3b69a40.html</t>
         </is>
       </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2024-10-26</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1060,6 +1295,11 @@
           <t>http://jud-anexos.digesto.com.br/b181fda9ca2e1a74482446c48f6d74de.html</t>
         </is>
       </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2024-11-25</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1073,6 +1313,11 @@
           <t>http://jud-anexos.digesto.com.br/4f9bfe3261339a4e4f8047b31d365c3e.html</t>
         </is>
       </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1086,6 +1331,11 @@
           <t>http://jud-anexos.digesto.com.br/4cae487ccb17bad14493add401f2fc1b.html</t>
         </is>
       </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2025-01-09</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1099,6 +1349,11 @@
           <t>http://jud-anexos.digesto.com.br/277a0743a7577dde103a227a6b5686b7.pdf</t>
         </is>
       </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2023-02-28</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -1112,6 +1367,11 @@
           <t>http://jud-anexos.digesto.com.br/8dce3b219c169bd525ef02a8b4929918.html</t>
         </is>
       </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2024-03-08</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1125,6 +1385,11 @@
           <t>http://jud-anexos.digesto.com.br/59e5eca3ab551ace1b54af92ffd89d30.html</t>
         </is>
       </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2024-12-16</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1138,6 +1403,11 @@
           <t>http://jud-anexos.digesto.com.br/5cafac9d036a7ae5bc0175281a13e604.html</t>
         </is>
       </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2025-01-23</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1151,6 +1421,11 @@
           <t>http://jud-anexos.digesto.com.br/b2c65a043aecb62d7790436432aa3bca.html</t>
         </is>
       </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2025-02-06</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -1164,6 +1439,11 @@
           <t>http://jud-anexos.digesto.com.br/339b138770633c32dc5bdb45dff360a7.html</t>
         </is>
       </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2025-01-22</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1177,6 +1457,11 @@
           <t>http://jud-anexos.digesto.com.br/4240158de62b97ae51c1d06c8a5cb8c2.html</t>
         </is>
       </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2024-11-27</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1190,6 +1475,11 @@
           <t>http://jud-anexos.digesto.com.br/ba7d733826bdefcd3324c783b812eff6.html</t>
         </is>
       </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2025-02-03</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -1203,6 +1493,11 @@
           <t>http://jud-anexos.digesto.com.br/e9a378d9c5c10e2dcbceffc83f4b4dcb.html</t>
         </is>
       </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2024-07-05</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -1216,6 +1511,11 @@
           <t>http://jud-anexos.digesto.com.br/a95e72b6484491d880d0c16548f1a788.html</t>
         </is>
       </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -1229,6 +1529,11 @@
           <t>http://jud-anexos.digesto.com.br/ae0f41bd0f206ab21b90f2edd13e3751.html</t>
         </is>
       </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2024-06-28</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -1242,6 +1547,11 @@
           <t>http://jud-anexos.digesto.com.br/179ce549bff6f6044d73c9c6f7b54d98.html</t>
         </is>
       </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2024-06-25</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -1255,6 +1565,11 @@
           <t>http://jud-anexos.digesto.com.br/77b0c057574bc4dbd51abea0e3970c3a.html</t>
         </is>
       </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2024-07-09</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -1268,6 +1583,11 @@
           <t>http://jud-anexos.digesto.com.br/a787730a033682f40bbaa5609b7e53ce.html</t>
         </is>
       </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2024-08-31</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -1281,6 +1601,11 @@
           <t>http://jud-anexos.digesto.com.br/e50aea65864c6a6ca7ab8ab06025d54f.pdf</t>
         </is>
       </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2017-04-05</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -1294,6 +1619,11 @@
           <t>http://jud-anexos.digesto.com.br/e50aea65864c6a6ca7ab8ab06025d54f.pdf</t>
         </is>
       </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2017-04-10</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -1307,6 +1637,11 @@
           <t>http://jud-anexos.digesto.com.br/433c23bd60fe494bb4c05e7166e4e75c.pdf</t>
         </is>
       </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2017-12-20</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -1320,6 +1655,11 @@
           <t>http://jud-anexos.digesto.com.br/c9c4529e46b75ee5e400e42350f2b2d7.pdf</t>
         </is>
       </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2016-05-04</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -1333,6 +1673,11 @@
           <t>http://jud-anexos.digesto.com.br/7492c259f2f14c410d044b4cda621a3e.pdf</t>
         </is>
       </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2016-12-19</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -1346,6 +1691,11 @@
           <t>http://jud-anexos.digesto.com.br/7b72c83d86eb82038f3a82a4ef007e73.pdf</t>
         </is>
       </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2019-12-04</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -1359,6 +1709,11 @@
           <t>http://jud-anexos.digesto.com.br/4a966dbc383fe11597026e3ca7432c93.pdf</t>
         </is>
       </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2024-04-15</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -1372,6 +1727,11 @@
           <t>http://jud-anexos.digesto.com.br/e0a197f13d29ce45ab6c10b51d54cce1.pdf</t>
         </is>
       </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2024-05-10</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -1385,6 +1745,11 @@
           <t>http://jud-anexos.digesto.com.br/2353a9d33244ebec151b2d9fe7f47749.html</t>
         </is>
       </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2022-04-28</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -1398,6 +1763,11 @@
           <t>http://jud-anexos.digesto.com.br/d6286211738884094ee30edb139f3179.html</t>
         </is>
       </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2024-03-07</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -1411,6 +1781,11 @@
           <t>http://jud-anexos.digesto.com.br/d87d77334f301639b1a30c4ce02bed40.html</t>
         </is>
       </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -1424,6 +1799,11 @@
           <t>http://jud-anexos.digesto.com.br/a8436eab252d9864569904719aa11a05.html</t>
         </is>
       </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2024-11-07</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -1437,6 +1817,11 @@
           <t>http://jud-anexos.digesto.com.br/e448073edc85a7c3dd335c89e2c64c2e.html</t>
         </is>
       </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2024-04-03</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -1450,6 +1835,11 @@
           <t>http://jud-anexos.digesto.com.br/4af9d082c1a6dd5841a9c871eb76b26b.html</t>
         </is>
       </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2024-01-24</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -1463,6 +1853,11 @@
           <t>http://jud-anexos.digesto.com.br/cbdda0e55f226a6f1eac06b4a819d143.html</t>
         </is>
       </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2024-07-01</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -1476,6 +1871,11 @@
           <t>http://jud-anexos.digesto.com.br/a782eb49096a58432ef4575eb778d2d9.pdf</t>
         </is>
       </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2019-02-28</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -1489,6 +1889,11 @@
           <t>http://jud-anexos.digesto.com.br/890c599772dcfc0dcc8a79de87894574.html</t>
         </is>
       </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2019-02-28</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -1502,6 +1907,11 @@
           <t>http://jud-anexos.digesto.com.br/ef234e8ea2b92676b43354833205ebc5.pdf</t>
         </is>
       </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2020-07-22</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -1515,6 +1925,11 @@
           <t>http://jud-anexos.digesto.com.br/dbfd6f128b5bf77b83af357d8688ae0a.html</t>
         </is>
       </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2024-09-29</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -1528,6 +1943,11 @@
           <t>http://jud-anexos.digesto.com.br/7ddaa644d9f08c8fb4d8cd9e145f54d8.html</t>
         </is>
       </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2024-10-15</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -1541,6 +1961,11 @@
           <t>http://jud-anexos.digesto.com.br/5db70668bded8052921d505ee0b45354.html</t>
         </is>
       </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2025-01-14</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -1554,6 +1979,11 @@
           <t>http://jud-anexos.digesto.com.br/a60b412bc2ec31a3cf504a884eae6a00.html</t>
         </is>
       </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2024-04-15</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -1567,6 +1997,11 @@
           <t>http://jud-anexos.digesto.com.br/15e1872c6fc17547f1f5684bfbd989de.html</t>
         </is>
       </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2024-10-04</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -1580,6 +2015,11 @@
           <t>http://jud-anexos.digesto.com.br/8d64e3a44693f0c1b6712febfdea5f57.html</t>
         </is>
       </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2024-08-14</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -1593,6 +2033,11 @@
           <t>http://jud-anexos.digesto.com.br/6a58c1d53ca40bba31fc16c058a9c823.html</t>
         </is>
       </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>2025-01-31</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -1606,6 +2051,11 @@
           <t>http://jud-anexos.digesto.com.br/29ade71890723450e4d7760765af7907.html</t>
         </is>
       </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>2024-12-05</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -1619,6 +2069,11 @@
           <t>http://jud-anexos.digesto.com.br/91a50d96fe4fd814562c4994b896c692.html</t>
         </is>
       </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>2024-09-16</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -1632,6 +2087,11 @@
           <t>http://jud-anexos.digesto.com.br/98c10db5b81fc04cc662aa2e9f9703e6.html</t>
         </is>
       </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>2025-01-17</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -1645,6 +2105,11 @@
           <t>http://jud-anexos.digesto.com.br/75797d6c643b50b94076a9abe92f8ca6.html</t>
         </is>
       </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>2025-02-20</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -1658,6 +2123,11 @@
           <t>http://jud-anexos.digesto.com.br/afe9bdf6acaff828b37f419d446ff634.html</t>
         </is>
       </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>2024-10-10</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -1671,6 +2141,11 @@
           <t>http://jud-anexos.digesto.com.br/3a9c242fe56e64fe7dda8b7f4185a774.html</t>
         </is>
       </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>2024-10-31</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -1684,6 +2159,11 @@
           <t>http://jud-anexos.digesto.com.br/f8965f4d8438a120c90429ed4958daa4.html</t>
         </is>
       </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>2025-01-09</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -1697,6 +2177,11 @@
           <t>http://jud-anexos.digesto.com.br/99bac9f8a27b6f863c8a701b23287cf1.html</t>
         </is>
       </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>2022-08-12</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -1710,6 +2195,11 @@
           <t>http://jud-anexos.digesto.com.br/894d562c0e6b878f1a5ca3e929cf4976.html</t>
         </is>
       </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>2022-08-15</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -1723,6 +2213,11 @@
           <t>http://jud-anexos.digesto.com.br/db1f453e0282f7b35bff833b8c3a8b26.html</t>
         </is>
       </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>2022-08-15</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -1736,6 +2231,11 @@
           <t>http://jud-anexos.digesto.com.br/ce8f59d9122482ea2e85fb2de0107b91.pdf</t>
         </is>
       </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>2022-09-16</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -1749,6 +2249,11 @@
           <t>http://jud-anexos.digesto.com.br/63b85b4704f36b0b1a95558eb6e23dfb.pdf</t>
         </is>
       </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>2023-02-06</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -1762,6 +2267,11 @@
           <t>http://jud-anexos.digesto.com.br/8afb384194c8d1bf4b0565c30c436910.html</t>
         </is>
       </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>2024-10-31</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -1775,6 +2285,11 @@
           <t>http://jud-anexos.digesto.com.br/8ac605d96900a316631cd68810d4cbc3.html</t>
         </is>
       </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>2024-11-16</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -1788,6 +2303,11 @@
           <t>http://jud-anexos.digesto.com.br/27b0dac944408c17fd8e67360baf2d6d.html</t>
         </is>
       </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>2025-03-12</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -1801,6 +2321,11 @@
           <t>http://jud-anexos.digesto.com.br/cf881aeec73b8b78fba6704f350cfbda.html</t>
         </is>
       </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>2023-11-30</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -1814,6 +2339,11 @@
           <t>http://jud-anexos.digesto.com.br/1dc5b67c98a0c4a0f05a009b155a3220.html</t>
         </is>
       </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>2024-09-17</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -1827,6 +2357,11 @@
           <t>http://jud-anexos.digesto.com.br/4414999b2fce2b47709c56598bf88f36.html</t>
         </is>
       </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>2025-02-28</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -1840,6 +2375,11 @@
           <t>http://jud-anexos.digesto.com.br/c040438bb09c42d719a6ea71a24722c2.html</t>
         </is>
       </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>2024-10-04</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -1853,6 +2393,11 @@
           <t>http://jud-anexos.digesto.com.br/45f47fefd2edbf68daf0b9145e7ef110.html</t>
         </is>
       </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>2022-06-06</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -1866,6 +2411,11 @@
           <t>http://jud-anexos.digesto.com.br/0c873297377df59bbca7198a8926b879.html</t>
         </is>
       </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>2022-10-10</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -1879,6 +2429,11 @@
           <t>http://jud-anexos.digesto.com.br/71e5a06de0a375326d4d9a327986aa08.html</t>
         </is>
       </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>2022-06-06</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -1892,6 +2447,11 @@
           <t>http://jud-anexos.digesto.com.br/5d13bef4f1d5c4f06444215079c749b2.html</t>
         </is>
       </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>2024-12-03</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -1905,6 +2465,11 @@
           <t>http://jud-anexos.digesto.com.br/4cdcb5f3961430b1fe3d15f1ddab6c10.html</t>
         </is>
       </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>2025-02-25</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -1918,6 +2483,11 @@
           <t>http://jud-anexos.digesto.com.br/861561d4e738b944ab9afdbc919939f7.html</t>
         </is>
       </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>2024-08-31</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -1931,6 +2501,11 @@
           <t>http://jud-anexos.digesto.com.br/56d0746e461568f3cff871358f0f5775.html</t>
         </is>
       </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>2024-12-02</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -1944,6 +2519,11 @@
           <t>http://jud-anexos.digesto.com.br/5d13bef4f1d5c4f06444215079c749b2.html</t>
         </is>
       </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>2024-12-03</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -1957,6 +2537,11 @@
           <t>http://jud-anexos.digesto.com.br/4cdcb5f3961430b1fe3d15f1ddab6c10.html</t>
         </is>
       </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>2025-02-25</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -1970,6 +2555,11 @@
           <t>http://jud-anexos.digesto.com.br/2f0f3617596191f9372b2324162a008d.html</t>
         </is>
       </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>2024-05-06</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -1983,6 +2573,11 @@
           <t>http://jud-anexos.digesto.com.br/8a006cdfd7b3a5954904d1d61efd0606.html</t>
         </is>
       </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>2025-03-28</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -1996,6 +2591,11 @@
           <t>http://jud-anexos.digesto.com.br/96f64175cf3048c46848c0b6e1d2c949.html</t>
         </is>
       </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -2009,6 +2609,11 @@
           <t>http://jud-anexos.digesto.com.br/482695eebfcaf32fda909f2c1602a7e0.html</t>
         </is>
       </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>2024-10-18</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -2022,6 +2627,11 @@
           <t>http://jud-anexos.digesto.com.br/9922dba4fa3aa19f537b33ceaf9cca3c.html</t>
         </is>
       </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>2024-10-31</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -2035,6 +2645,11 @@
           <t>http://jud-anexos.digesto.com.br/7d9dc3b4f3cc872992d2dce50336a1a8.html</t>
         </is>
       </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>2024-05-02</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -2048,6 +2663,11 @@
           <t>http://jud-anexos.digesto.com.br/fdf122349fdec9073c628cfd314fe90e.html</t>
         </is>
       </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>2024-05-24</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -2061,6 +2681,11 @@
           <t>http://jud-anexos.digesto.com.br/0f2d38c2bb59126460be17901b5a05e4.html</t>
         </is>
       </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>2024-06-10</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -2074,6 +2699,11 @@
           <t>http://jud-anexos.digesto.com.br/2cf3a27a1758e5e20803d4402b368ebd.html</t>
         </is>
       </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>2024-10-10</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -2087,6 +2717,11 @@
           <t>http://jud-anexos.digesto.com.br/bb7c46ec40d014732e9e97f1b64694b9.html</t>
         </is>
       </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>2024-12-06</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -2100,6 +2735,11 @@
           <t>http://jud-anexos.digesto.com.br/03f0ea17d462af0092970c2e13962dbf.html</t>
         </is>
       </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>2024-09-18</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -2113,6 +2753,11 @@
           <t>http://jud-anexos.digesto.com.br/e8c7d9c59693b9cdf82fab464338387a.html</t>
         </is>
       </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>2024-09-23</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -2126,6 +2771,11 @@
           <t>http://jud-anexos.digesto.com.br/f1e5b6f5606c57c13faf42207431d2ef.html</t>
         </is>
       </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>2024-08-13</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -2139,6 +2789,11 @@
           <t>http://jud-anexos.digesto.com.br/e748a98ec567a8446cf05d6974c9d6d5.html</t>
         </is>
       </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>2025-01-31</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -2152,6 +2807,11 @@
           <t>http://jud-anexos.digesto.com.br/787aac910b0ccc1f7883b2df4291b2cd.html</t>
         </is>
       </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>2024-08-20</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
@@ -2165,6 +2825,11 @@
           <t>http://jud-anexos.digesto.com.br/18818cc18d5c33897d8a6aa0bc515dc9.pdf</t>
         </is>
       </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>2024-08-05</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
@@ -2178,6 +2843,11 @@
           <t>http://jud-anexos.digesto.com.br/7ef000358177fe817f11a89252d6eab3.pdf</t>
         </is>
       </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>2024-08-05</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -2191,6 +2861,11 @@
           <t>http://jud-anexos.digesto.com.br/bf59084f6e8958074ae8a88807f76da0.html</t>
         </is>
       </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>2024-08-05</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -2204,6 +2879,11 @@
           <t>http://jud-anexos.digesto.com.br/a894223ac9c87f6fe5b359beed4cbb82.pdf</t>
         </is>
       </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>2024-08-05</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -2217,6 +2897,11 @@
           <t>http://jud-anexos.digesto.com.br/5c17440bf0797434ce61ca483ad31a2b.pdf</t>
         </is>
       </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>2024-08-05</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -2230,6 +2915,11 @@
           <t>http://jud-anexos.digesto.com.br/1eba2a18d3f4887800d0b3df170a2301.html</t>
         </is>
       </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>2024-08-05</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -2243,6 +2933,11 @@
           <t>http://jud-anexos.digesto.com.br/02597b35d5e8ece30d36627f30550386.html</t>
         </is>
       </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>2020-01-23</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -2256,6 +2951,11 @@
           <t>http://jud-anexos.digesto.com.br/2f94e35b8b781886a8989761ab7b9e54.html</t>
         </is>
       </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>2021-03-03</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -2269,6 +2969,11 @@
           <t>http://jud-anexos.digesto.com.br/7d54d2fd28f74c625bb2157b3d507fe6.html</t>
         </is>
       </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>2023-01-30</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -2282,6 +2987,11 @@
           <t>http://jud-anexos.digesto.com.br/5cd0f358f60916910c4ce7a1d77bc41d.html</t>
         </is>
       </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>2023-03-20</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -2295,6 +3005,11 @@
           <t>http://jud-anexos.digesto.com.br/fab3efa39a57f1d1a8bd1457980931ab.html</t>
         </is>
       </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>2023-12-04</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -2308,6 +3023,11 @@
           <t>http://jud-anexos.digesto.com.br/b245bb859068c487a5f72daf3b444ea6.pdf</t>
         </is>
       </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>2022-12-14</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -2321,6 +3041,11 @@
           <t>http://jud-anexos.digesto.com.br/5d986cf505b92ed91f16c175e1f3e8bc.html</t>
         </is>
       </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>2022-12-14</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -2334,6 +3059,11 @@
           <t>http://jud-anexos.digesto.com.br/a8969889a4297e9be4801b77864e0072.pdf</t>
         </is>
       </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>2023-11-03</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -2347,6 +3077,11 @@
           <t>http://jud-anexos.digesto.com.br/a86eb3b515c13807621a2034f22634f6.html</t>
         </is>
       </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>2023-11-03</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -2360,6 +3095,11 @@
           <t>http://jud-anexos.digesto.com.br/aa4a5320947278386333bfae47987ed3.pdf</t>
         </is>
       </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>2023-11-24</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
@@ -2373,6 +3113,11 @@
           <t>http://jud-anexos.digesto.com.br/9c4720025145e7c89829a5e2b0a65112.html</t>
         </is>
       </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>2023-11-24</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -2386,6 +3131,11 @@
           <t>http://jud-anexos.digesto.com.br/eabd85570883cfb002cdd7cd4b360502.pdf</t>
         </is>
       </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>2024-01-22</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -2399,6 +3149,11 @@
           <t>http://jud-anexos.digesto.com.br/7a40f6e8360a2ab863c48335ba43f58f.html</t>
         </is>
       </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>2024-06-13</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
@@ -2412,6 +3167,11 @@
           <t>http://jud-anexos.digesto.com.br/af54e0b0f9b10f004a73f2c6d5216a46.pdf</t>
         </is>
       </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>2024-08-05</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -2425,6 +3185,11 @@
           <t>http://jud-anexos.digesto.com.br/39a92dda8213d3adf1e0c278c9d3d426.pdf</t>
         </is>
       </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -2438,6 +3203,11 @@
           <t>http://jud-anexos.digesto.com.br/c17569a429370248eb4a640d89e6305f.html</t>
         </is>
       </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>2025-02-26</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
@@ -2451,6 +3221,11 @@
           <t>http://jud-anexos.digesto.com.br/0b30088042a5e4b14b46f0c9114aeee0.html</t>
         </is>
       </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>2022-03-14</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -2464,6 +3239,11 @@
           <t>http://jud-anexos.digesto.com.br/e7eaa69d4998650a8778720bcd2124b1.pdf</t>
         </is>
       </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>2023-02-06</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -2477,6 +3257,11 @@
           <t>http://jud-anexos.digesto.com.br/4aecb6e4be9b62dd61fd3fa94216f1c7.pdf</t>
         </is>
       </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>2023-06-21</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -2490,6 +3275,11 @@
           <t>http://jud-anexos.digesto.com.br/aad4c08af0fed2a59ac21cdfe0f2d09d.html</t>
         </is>
       </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>2023-07-11</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -2503,6 +3293,11 @@
           <t>http://jud-anexos.digesto.com.br/49852b745995b4c8e6eaf169d8a7b0ab.pdf</t>
         </is>
       </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>2023-07-26</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
@@ -2516,6 +3311,11 @@
           <t>http://jud-anexos.digesto.com.br/af3466096800dc2c18bfb6ce0091e157.pdf</t>
         </is>
       </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>2024-12-19</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -2529,6 +3329,11 @@
           <t>http://jud-anexos.digesto.com.br/482c0356106afbc8fbe19a09dd3a18c8.html</t>
         </is>
       </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>2025-03-03</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -2542,6 +3347,11 @@
           <t>http://jud-anexos.digesto.com.br/b78e3f7661c147479312174922ebd54a.html</t>
         </is>
       </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>2025-02-21</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
@@ -2555,6 +3365,11 @@
           <t>http://jud-anexos.digesto.com.br/aa53709a02c99c33027e30faa5cc3c4a.html</t>
         </is>
       </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>2024-09-19</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
@@ -2568,6 +3383,11 @@
           <t>http://jud-anexos.digesto.com.br/c162a3e8ba8102753bf507c27416a779.html</t>
         </is>
       </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>2024-09-20</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -2581,6 +3401,11 @@
           <t>http://jud-anexos.digesto.com.br/3e913727aa87d253f06d2d841e0ac43d.html</t>
         </is>
       </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>2024-11-11</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -2594,6 +3419,11 @@
           <t>http://jud-anexos.digesto.com.br/ef958017381814c5e3e7f0acdee348d8.html</t>
         </is>
       </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -2607,6 +3437,11 @@
           <t>http://jud-anexos.digesto.com.br/c536491278daffd551de30a3a89b0077.html</t>
         </is>
       </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -2620,6 +3455,11 @@
           <t>http://jud-anexos.digesto.com.br/069bd0928907f2adb9d7ca4e9fdcdb9e.pdf</t>
         </is>
       </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -2633,6 +3473,11 @@
           <t>http://jud-anexos.digesto.com.br/114c8d4e727e334fbc2bc86bcc52198a.html</t>
         </is>
       </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
@@ -2646,6 +3491,11 @@
           <t>http://jud-anexos.digesto.com.br/8b618f6647f96165a3decaf7a2dc35dd.pdf</t>
         </is>
       </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
@@ -2659,6 +3509,11 @@
           <t>http://jud-anexos.digesto.com.br/b014fe9d2ab51224e0e514c5cc4c0dce.pdf</t>
         </is>
       </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
@@ -2672,6 +3527,11 @@
           <t>http://jud-anexos.digesto.com.br/bd9407845c00232e3c0b70823b43f0a9.html</t>
         </is>
       </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
@@ -2685,6 +3545,11 @@
           <t>http://jud-anexos.digesto.com.br/9fd5c28ae932d7c91cd943895a908874.html</t>
         </is>
       </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>2023-11-20</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
@@ -2698,6 +3563,11 @@
           <t>http://jud-anexos.digesto.com.br/ccb283525ccc3117ede60f699789d717.html</t>
         </is>
       </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
@@ -2711,6 +3581,11 @@
           <t>http://jud-anexos.digesto.com.br/2d4167fb6263394d4638e8f17684666a.html</t>
         </is>
       </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>2023-12-01</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
@@ -2724,6 +3599,11 @@
           <t>http://jud-anexos.digesto.com.br/d538a5f227eb2f85ed7c500bcc990b84.html</t>
         </is>
       </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>2023-09-19</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
@@ -2737,6 +3617,11 @@
           <t>http://jud-anexos.digesto.com.br/c81a352e5496d1bf8997ba7722c96f6d.html</t>
         </is>
       </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>2025-02-05</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
@@ -2750,6 +3635,11 @@
           <t>http://jud-anexos.digesto.com.br/d53473669e32bba5d53f01f1275c456c.html</t>
         </is>
       </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>2022-01-10</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
@@ -2763,6 +3653,11 @@
           <t>http://jud-anexos.digesto.com.br/c2838924671d21e2205937f14516cc52.html</t>
         </is>
       </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>2020-07-13</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
@@ -2776,6 +3671,11 @@
           <t>http://jud-anexos.digesto.com.br/bb16177ec388ee88c102e0459cd3daf0.pdf</t>
         </is>
       </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>2024-07-24</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
@@ -2789,6 +3689,11 @@
           <t>http://jud-anexos.digesto.com.br/466086751c0b018d394268a9d4216e02.pdf</t>
         </is>
       </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
@@ -2802,6 +3707,11 @@
           <t>http://jud-anexos.digesto.com.br/73fd817299d1c63c88854034bfcc8a4a.pdf</t>
         </is>
       </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
@@ -2815,6 +3725,11 @@
           <t>http://jud-anexos.digesto.com.br/cc45996fbc5147e18ac5b233bb930927.pdf</t>
         </is>
       </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
@@ -2828,6 +3743,11 @@
           <t>http://jud-anexos.digesto.com.br/bb0f8570928008e3328bcb8fe3347ff0.pdf</t>
         </is>
       </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>2025-01-22</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
@@ -2841,6 +3761,11 @@
           <t>http://jud-anexos.digesto.com.br/385da7ae2e6c0c651b4d4c0940472edf.html</t>
         </is>
       </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>2024-12-18</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
@@ -2854,6 +3779,11 @@
           <t>http://jud-anexos.digesto.com.br/53b7e3de858eaa2909080dcd4c5b2ffc.html</t>
         </is>
       </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>2024-10-04</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
@@ -2867,6 +3797,11 @@
           <t>http://jud-anexos.digesto.com.br/4920bbc7514401947b53d167eeede610.html</t>
         </is>
       </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>2024-06-13</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
@@ -2880,6 +3815,11 @@
           <t>http://jud-anexos.digesto.com.br/f67083d1cd67470cf74924563c181e62.html</t>
         </is>
       </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>2022-02-16</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
@@ -2893,6 +3833,11 @@
           <t>http://jud-anexos.digesto.com.br/593fdde07807a09bbf703d326f0d520b.pdf</t>
         </is>
       </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>2022-02-16</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
@@ -2906,6 +3851,11 @@
           <t>http://jud-anexos.digesto.com.br/a40e94643357c64d5b6e9995cd5b4763.html</t>
         </is>
       </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>2022-02-16</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
@@ -2919,6 +3869,11 @@
           <t>http://jud-anexos.digesto.com.br/f78bbe35bc536988e3f48991a8391983.html</t>
         </is>
       </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>2022-09-29</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
@@ -2932,6 +3887,11 @@
           <t>http://jud-anexos.digesto.com.br/c3fd78c0600d0685977a9276d9791bb9.pdf</t>
         </is>
       </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>2022-09-29</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
@@ -2945,6 +3905,11 @@
           <t>http://jud-anexos.digesto.com.br/b54b43e57133d78e16822e1f8607d90f.html</t>
         </is>
       </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>2022-09-29</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
@@ -2958,6 +3923,11 @@
           <t>http://jud-anexos.digesto.com.br/4c4d58cac4ce5b58e5d1a25415c7e915.html</t>
         </is>
       </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>2023-05-09</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
@@ -2971,6 +3941,11 @@
           <t>http://jud-anexos.digesto.com.br/8a2953171e41dfe3702677a35bc2200e.html</t>
         </is>
       </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>2023-05-15</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
@@ -2984,6 +3959,11 @@
           <t>http://jud-anexos.digesto.com.br/a3b072000b3601095e081cb7f4f29d7a.pdf</t>
         </is>
       </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>2024-03-07</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
@@ -2997,6 +3977,11 @@
           <t>http://jud-anexos.digesto.com.br/542cef14fa601e8e73a2bba292d8918d.pdf</t>
         </is>
       </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>2023-11-06</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
@@ -3010,6 +3995,11 @@
           <t>http://jud-anexos.digesto.com.br/1647576dbabeccdd2efc2e99a67bebb5.html</t>
         </is>
       </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>2023-11-06</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
@@ -3023,6 +4013,11 @@
           <t>http://jud-anexos.digesto.com.br/5ba5dbc98cc98ffd3ff6f2ea0d623328.pdf</t>
         </is>
       </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>2023-11-06</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
@@ -3036,6 +4031,11 @@
           <t>http://jud-anexos.digesto.com.br/937d52ca03546c6953172e1872148a05.html</t>
         </is>
       </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>2023-11-06</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
@@ -3049,6 +4049,11 @@
           <t>http://jud-anexos.digesto.com.br/b5ce31b71387ce456613bf9c035c9186.html</t>
         </is>
       </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>2023-11-06</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
@@ -3062,6 +4067,11 @@
           <t>http://jud-anexos.digesto.com.br/e6f6fcec3ee1e610cefc85f7fe16475c.html</t>
         </is>
       </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>2023-11-13</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
@@ -3075,6 +4085,11 @@
           <t>http://jud-anexos.digesto.com.br/14f4eed10d9b11c0a52e9a7ea12e1353.html</t>
         </is>
       </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
@@ -3088,6 +4103,11 @@
           <t>http://jud-anexos.digesto.com.br/8f0882a5139a55648c081c81efebd249.html</t>
         </is>
       </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
@@ -3101,6 +4121,11 @@
           <t>http://jud-anexos.digesto.com.br/c4ef928d4c5550778b98802ffa9115ec.pdf</t>
         </is>
       </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>2024-05-14</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
@@ -3114,6 +4139,11 @@
           <t>http://jud-anexos.digesto.com.br/464f73c7fc4d8f0d46dab27b4052c5e8.html</t>
         </is>
       </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>2021-01-15</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
@@ -3127,6 +4157,11 @@
           <t>http://jud-anexos.digesto.com.br/b429b8c72a7e0fe233228a06312116de.html</t>
         </is>
       </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>2021-01-15</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
@@ -3140,6 +4175,11 @@
           <t>http://jud-anexos.digesto.com.br/e1dda60d3cd0068baf7608d97577f6f8.html</t>
         </is>
       </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>2024-09-04</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
@@ -3153,6 +4193,11 @@
           <t>http://jud-anexos.digesto.com.br/50f8841326f8a8fe3f0b97ae189e21f2.pdf</t>
         </is>
       </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>2023-04-24</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
@@ -3166,6 +4211,11 @@
           <t>http://jud-anexos.digesto.com.br/43ce932ede7913be7bb8aaf445a6cf86.pdf</t>
         </is>
       </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>2023-02-16</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
@@ -3179,6 +4229,11 @@
           <t>http://jud-anexos.digesto.com.br/43ce932ede7913be7bb8aaf445a6cf86.pdf</t>
         </is>
       </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>2023-02-16</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
@@ -3192,6 +4247,11 @@
           <t>http://jud-anexos.digesto.com.br/ee8d4ccd9502acf493dddad0ff624099.pdf</t>
         </is>
       </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>2018-07-12</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
@@ -3205,6 +4265,11 @@
           <t>http://jud-anexos.digesto.com.br/ee8d4ccd9502acf493dddad0ff624099.pdf</t>
         </is>
       </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>2018-07-17</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
@@ -3218,6 +4283,11 @@
           <t>http://jud-anexos.digesto.com.br/ac533c682460fc6b9238f88428293f5e.html</t>
         </is>
       </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>2020-09-23</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
@@ -3231,6 +4301,11 @@
           <t>http://jud-anexos.digesto.com.br/cc378e246e9f2bb624e39c5f44cba5ea.html</t>
         </is>
       </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>2020-09-23</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
@@ -3244,6 +4319,11 @@
           <t>http://jud-anexos.digesto.com.br/b8e8c4a5649c41ff0423d6d783fe9e6e.html</t>
         </is>
       </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>2024-04-15</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
@@ -3257,6 +4337,11 @@
           <t>http://jud-anexos.digesto.com.br/406aba7ce0f1a766e399fc8a6b426e92.html</t>
         </is>
       </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>2024-10-07</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
@@ -3270,6 +4355,11 @@
           <t>http://jud-anexos.digesto.com.br/59b91ee286ab5e6789bbbd35ecc00e18.html</t>
         </is>
       </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>2023-10-27</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
@@ -3283,6 +4373,11 @@
           <t>http://jud-anexos.digesto.com.br/d22bae16ffd990c5f2778f6a2fdc1c9d.html</t>
         </is>
       </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>2024-06-12</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
@@ -3296,6 +4391,11 @@
           <t>http://jud-anexos.digesto.com.br/f2aec7d1178b67dfa5f261f370369331.pdf</t>
         </is>
       </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>2024-06-14</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
@@ -3309,6 +4409,11 @@
           <t>http://jud-anexos.digesto.com.br/7e8ef9ce032dd9a17851de896af3c3ab.html</t>
         </is>
       </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>2024-06-14</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
@@ -3322,6 +4427,11 @@
           <t>http://jud-anexos.digesto.com.br/05f6c7cd3bc73041620357c6951529f6.html</t>
         </is>
       </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>2024-06-14</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
@@ -3335,6 +4445,11 @@
           <t>http://jud-anexos.digesto.com.br/801f2566cef0933e273ea0f32cfbf20b.pdf</t>
         </is>
       </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>2024-06-14</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
@@ -3348,6 +4463,11 @@
           <t>http://jud-anexos.digesto.com.br/979e322edba8d95025dad85bbce31c49.html</t>
         </is>
       </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>2024-06-14</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
@@ -3361,6 +4481,11 @@
           <t>http://jud-anexos.digesto.com.br/2465d51bbfb11dd100ff2d7d7abbdecd.html</t>
         </is>
       </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>2024-11-06</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
@@ -3374,6 +4499,11 @@
           <t>http://jud-anexos.digesto.com.br/be29c15615df1088aa4f8e4abd8e9171.html</t>
         </is>
       </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>2024-05-16</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
@@ -3387,6 +4517,11 @@
           <t>http://jud-anexos.digesto.com.br/d6421e9158a620e3a296b16e215dbdb8.html</t>
         </is>
       </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>2024-07-17</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
@@ -3400,6 +4535,11 @@
           <t>http://jud-anexos.digesto.com.br/413fbebff2bec44a857c5b3f74e93c13.pdf</t>
         </is>
       </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>2023-09-22</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
@@ -3413,6 +4553,11 @@
           <t>http://jud-anexos.digesto.com.br/413fbebff2bec44a857c5b3f74e93c13.pdf</t>
         </is>
       </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>2023-09-28</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
@@ -3426,6 +4571,11 @@
           <t>http://jud-anexos.digesto.com.br/98af04439c32a3f01cab92368b24e9f6.pdf</t>
         </is>
       </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>2024-10-09</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
@@ -3439,6 +4589,11 @@
           <t>http://jud-anexos.digesto.com.br/1a85bcce660ac9edd78b80f0c6c4f385.pdf</t>
         </is>
       </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
@@ -3452,6 +4607,11 @@
           <t>http://jud-anexos.digesto.com.br/1a85bcce660ac9edd78b80f0c6c4f385.pdf</t>
         </is>
       </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>2024-06-04</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
@@ -3465,6 +4625,11 @@
           <t>http://jud-anexos.digesto.com.br/bb942e80e50370a8ce615ee916b6be60.pdf</t>
         </is>
       </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>2024-06-23</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
@@ -3478,6 +4643,11 @@
           <t>http://jud-anexos.digesto.com.br/36775b0c027fa6f159465b2d2f841002.pdf</t>
         </is>
       </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>2024-09-05</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
@@ -3491,6 +4661,11 @@
           <t>http://jud-anexos.digesto.com.br/36775b0c027fa6f159465b2d2f841002.pdf</t>
         </is>
       </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>2024-09-05</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
@@ -3504,6 +4679,11 @@
           <t>http://jud-anexos.digesto.com.br/d4307d87fd4967ab91d1553bddc6315e.pdf</t>
         </is>
       </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>2024-03-26</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
@@ -3517,6 +4697,11 @@
           <t>http://jud-anexos.digesto.com.br/c1541200bd444765f2ceab1bcb73e591.pdf</t>
         </is>
       </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>2024-08-20</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
@@ -3530,6 +4715,11 @@
           <t>http://jud-anexos.digesto.com.br/a6d96720754eb540da89b0c074289ab4.pdf</t>
         </is>
       </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
@@ -3543,6 +4733,11 @@
           <t>http://jud-anexos.digesto.com.br/6064f2eaceb990ce89edf295ee40abbb.html</t>
         </is>
       </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
@@ -3556,6 +4751,11 @@
           <t>http://jud-anexos.digesto.com.br/50632273a0ca7e919478ecf9b4967371.pdf</t>
         </is>
       </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
@@ -3569,6 +4769,11 @@
           <t>http://jud-anexos.digesto.com.br/8aa938577e02cf5ca814dd987b892757.html</t>
         </is>
       </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>2024-06-05</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
@@ -3582,6 +4787,11 @@
           <t>http://jud-anexos.digesto.com.br/ec06640f48df305bd720a3462f3e422d.pdf</t>
         </is>
       </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
@@ -3595,6 +4805,11 @@
           <t>http://jud-anexos.digesto.com.br/62ba97dacf00dace69193bfecaf68c08.html</t>
         </is>
       </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
@@ -3608,6 +4823,11 @@
           <t>http://jud-anexos.digesto.com.br/35e71a948b35f2793c91cf08bf21b3a6.pdf</t>
         </is>
       </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>2024-09-10</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
@@ -3621,6 +4841,11 @@
           <t>http://jud-anexos.digesto.com.br/f685cd2ac497bcf48cc144fda9e3080a.html</t>
         </is>
       </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>2024-09-10</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
@@ -3634,6 +4859,11 @@
           <t>http://jud-anexos.digesto.com.br/537574a3d35619b67306100ce38ffd00.pdf</t>
         </is>
       </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
@@ -3647,6 +4877,11 @@
           <t>http://jud-anexos.digesto.com.br/6ad25c800f4bc36e5d622cf7b3cd6b9f.pdf</t>
         </is>
       </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>2024-07-25</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
@@ -3660,6 +4895,11 @@
           <t>http://jud-anexos.digesto.com.br/db945258b703695237d684917ef9df82.pdf</t>
         </is>
       </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>2017-08-31</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
@@ -3673,6 +4913,11 @@
           <t>http://jud-anexos.digesto.com.br/b67f279f0e5ad8f369817a33db0ae4d5.html</t>
         </is>
       </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>2022-04-27</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
@@ -3686,6 +4931,11 @@
           <t>http://jud-anexos.digesto.com.br/b6f974be79028fffcb09365724838968.pdf</t>
         </is>
       </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>2021-01-01</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
@@ -3699,6 +4949,11 @@
           <t>http://jud-anexos.digesto.com.br/d3a1117f9d7ff7de9773360348b31ab7.html</t>
         </is>
       </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>2023-05-03</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
@@ -3712,6 +4967,11 @@
           <t>http://jud-anexos.digesto.com.br/436d43f264f3615808ff79fff02fe4b5.html</t>
         </is>
       </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>2023-05-03</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
@@ -3725,6 +4985,11 @@
           <t>http://jud-anexos.digesto.com.br/2f54592eb832bf2c937d8333adb9730b.html</t>
         </is>
       </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>2024-09-17</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
@@ -3738,6 +5003,11 @@
           <t>http://jud-anexos.digesto.com.br/3b8c6d37c6eb69bc9b73a364ef4f989d.html</t>
         </is>
       </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>2024-09-17</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
@@ -3751,6 +5021,11 @@
           <t>http://jud-anexos.digesto.com.br/ad976e187beb75a00056c1c798c5e05c.html</t>
         </is>
       </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>2024-05-28</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
@@ -3764,6 +5039,11 @@
           <t>http://jud-anexos.digesto.com.br/e7a084af642050575078635fd07a8207.html</t>
         </is>
       </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>2024-03-26</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
@@ -3777,6 +5057,11 @@
           <t>http://jud-anexos.digesto.com.br/b4aa31f9b5ad3d2e7d87f1d44e2c22c6.html</t>
         </is>
       </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>2024-04-11</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
@@ -3790,6 +5075,11 @@
           <t>http://jud-anexos.digesto.com.br/db48a69c39c3d1750e471034af20807d.html</t>
         </is>
       </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>2023-04-11</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
@@ -3803,6 +5093,11 @@
           <t>http://jud-anexos.digesto.com.br/ba4a13581fbd7201f973284b43b7ab73.html</t>
         </is>
       </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>2023-08-23</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
@@ -3816,6 +5111,11 @@
           <t>http://jud-anexos.digesto.com.br/ad7c3a1522e86a30f90aaba33afb5388.pdf</t>
         </is>
       </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>2023-09-21</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
@@ -3829,6 +5129,11 @@
           <t>http://jud-anexos.digesto.com.br/f4db43bfa83c11e044e88e74b31f64c8.html</t>
         </is>
       </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>2021-02-22</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
@@ -3842,6 +5147,11 @@
           <t>http://jud-anexos.digesto.com.br/96672b35cf13cd89968acd66db14239e.pdf</t>
         </is>
       </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>2021-03-17</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
@@ -3855,6 +5165,11 @@
           <t>http://jud-anexos.digesto.com.br/dfd3140bf0bd0cd889a758169978fa85.pdf</t>
         </is>
       </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>2021-03-17</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
@@ -3868,6 +5183,11 @@
           <t>http://jud-anexos.digesto.com.br/2b26d5e67287be7cc7955949201fa2df.pdf</t>
         </is>
       </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>2021-03-17</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
@@ -3881,6 +5201,11 @@
           <t>http://jud-anexos.digesto.com.br/01ce5b4819ad565d7a72a05f5ea83f8f.html</t>
         </is>
       </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>2021-03-17</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
@@ -3894,6 +5219,11 @@
           <t>http://jud-anexos.digesto.com.br/914202522c22955d1f4442ccf27a7e3d.pdf</t>
         </is>
       </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>2022-08-16</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
@@ -3907,6 +5237,11 @@
           <t>http://jud-anexos.digesto.com.br/b21ed47b54ee3e8bb0a40e5cf5455c91.pdf</t>
         </is>
       </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>2022-08-16</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
@@ -3920,6 +5255,11 @@
           <t>http://jud-anexos.digesto.com.br/ff48371e3a37f1ee02ae4f6e4cbc7042.html</t>
         </is>
       </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>2022-08-16</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
@@ -3933,6 +5273,11 @@
           <t>http://jud-anexos.digesto.com.br/2d9e7d2bdd759b8d06ff0d0f6549cf4a.html</t>
         </is>
       </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>2023-11-20</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
@@ -3946,6 +5291,11 @@
           <t>http://jud-anexos.digesto.com.br/007e2b540150a8a72dffb18e31979031.pdf</t>
         </is>
       </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>2023-12-07</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
@@ -3959,6 +5309,11 @@
           <t>http://jud-anexos.digesto.com.br/54cb976b99dfc0aeb131a12c19332e48.pdf</t>
         </is>
       </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>2024-06-08</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
@@ -3972,6 +5327,11 @@
           <t>http://jud-anexos.digesto.com.br/253e356c5b91632c3b73619a56f1767f.pdf</t>
         </is>
       </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>2019-11-26</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="n">
@@ -3985,6 +5345,11 @@
           <t>http://jud-anexos.digesto.com.br/c1d25a940c174134e395b6b94dd1950d.pdf</t>
         </is>
       </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>2016-04-18</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
@@ -3998,6 +5363,11 @@
           <t>http://jud-anexos.digesto.com.br/f67a531415de88bd064371136e20f4e3.pdf</t>
         </is>
       </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>2016-11-23</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
@@ -4011,6 +5381,11 @@
           <t>http://jud-anexos.digesto.com.br/b5d68ab6d4a664a0bf59cc226ab09749.html</t>
         </is>
       </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>2020-06-15</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
@@ -4024,6 +5399,11 @@
           <t>http://jud-anexos.digesto.com.br/d292a628c22d1b32408ab79a90ed010d.html</t>
         </is>
       </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>2024-11-28</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
@@ -4037,6 +5417,11 @@
           <t>http://jud-anexos.digesto.com.br/84ad675b496f4358a11b4c46a85f947e.html</t>
         </is>
       </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>2024-09-16</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
@@ -4050,6 +5435,11 @@
           <t>http://jud-anexos.digesto.com.br/77480e191df61d24e27bdece4f05aa96.html</t>
         </is>
       </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>2024-10-22</t>
+        </is>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
@@ -4063,6 +5453,11 @@
           <t>http://jud-anexos.digesto.com.br/36b87731e8588b9710a4b71f764682b7.html</t>
         </is>
       </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>2024-10-16</t>
+        </is>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
@@ -4076,6 +5471,11 @@
           <t>http://jud-anexos.digesto.com.br/2c631fb82f4e1cf8e2943e9ce7857698.html</t>
         </is>
       </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>2025-01-10</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
@@ -4089,6 +5489,11 @@
           <t>http://jud-anexos.digesto.com.br/bb05fbed2d68e63768214d81c73ce946.html</t>
         </is>
       </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>2024-07-23</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
@@ -4102,6 +5507,11 @@
           <t>http://jud-anexos.digesto.com.br/b0239a024ea97a4776993220c67faced.pdf</t>
         </is>
       </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>2024-03-05</t>
+        </is>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
@@ -4115,6 +5525,11 @@
           <t>http://jud-anexos.digesto.com.br/a7e7d6002b57da000cb8b70078745cf0.pdf</t>
         </is>
       </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>2024-07-10</t>
+        </is>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
@@ -4128,6 +5543,11 @@
           <t>http://jud-anexos.digesto.com.br/d6d6c3d07b36e339a715713cd2a9f5e5.pdf</t>
         </is>
       </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>2024-04-11</t>
+        </is>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
@@ -4141,6 +5561,11 @@
           <t>http://jud-anexos.digesto.com.br/b2363de79263de171e7d2b5f9a8571b3.pdf</t>
         </is>
       </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>2024-04-23</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
@@ -4154,6 +5579,11 @@
           <t>http://jud-anexos.digesto.com.br/cb226c03e5d1ceb3d951835f40864109.html</t>
         </is>
       </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>2024-04-23</t>
+        </is>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
@@ -4167,6 +5597,11 @@
           <t>http://jud-anexos.digesto.com.br/51bb3bd00d9fb701967f9d974589ee9c.pdf</t>
         </is>
       </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>2022-07-19</t>
+        </is>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
@@ -4180,6 +5615,11 @@
           <t>http://jud-anexos.digesto.com.br/23e081a037c71eaef0985594bbf382b5.pdf</t>
         </is>
       </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>2022-05-30</t>
+        </is>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
@@ -4193,6 +5633,11 @@
           <t>http://jud-anexos.digesto.com.br/358ab5ff1d111711372796c49fb56929.pdf</t>
         </is>
       </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>2023-12-15</t>
+        </is>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="n">
@@ -4206,6 +5651,11 @@
           <t>http://jud-anexos.digesto.com.br/c1b371e8de959663e74bfc0565bd360d.pdf</t>
         </is>
       </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>2024-06-06</t>
+        </is>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
@@ -4219,6 +5669,11 @@
           <t>http://jud-anexos.digesto.com.br/225962d7d1434057c48cfe1e5124b9fe.pdf</t>
         </is>
       </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>2024-10-10</t>
+        </is>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
@@ -4232,6 +5687,11 @@
           <t>http://jud-anexos.digesto.com.br/fe31eb8b2b0ad867a6669c0a9226e51a.pdf</t>
         </is>
       </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>2019-04-25</t>
+        </is>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="n">
@@ -4245,6 +5705,11 @@
           <t>http://jud-anexos.digesto.com.br/6b0828e58be5ad4132e585d912e11c1f.pdf</t>
         </is>
       </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>2022-04-18</t>
+        </is>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
@@ -4258,6 +5723,11 @@
           <t>http://jud-anexos.digesto.com.br/ae3153b4e67c8424c8f84dd5f0c6905e.pdf</t>
         </is>
       </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>2024-12-12</t>
+        </is>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
@@ -4271,6 +5741,11 @@
           <t>http://jud-anexos.digesto.com.br/c466c60c12c8695b860c774071015352.pdf</t>
         </is>
       </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>2018-07-31</t>
+        </is>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
@@ -4284,6 +5759,11 @@
           <t>http://jud-anexos.digesto.com.br/75330423d1bacd4744138317fced1741.pdf</t>
         </is>
       </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>2021-06-08</t>
+        </is>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
@@ -4297,6 +5777,11 @@
           <t>http://jud-anexos.digesto.com.br/37b7bcd8b81b4c039f1e046737350d76.pdf</t>
         </is>
       </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>2021-08-05</t>
+        </is>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
@@ -4310,6 +5795,11 @@
           <t>http://jud-anexos.digesto.com.br/26881543f32c891c045ba0cd6786a952.pdf</t>
         </is>
       </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>2022-08-24</t>
+        </is>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
@@ -4323,6 +5813,11 @@
           <t>http://jud-anexos.digesto.com.br/e1d2d8461e91b4e7926b9fac09f65173.pdf</t>
         </is>
       </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>2021-10-22</t>
+        </is>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
@@ -4336,6 +5831,11 @@
           <t>http://jud-anexos.digesto.com.br/2e94cd8125a850b70179e36e1f3dc0be.pdf</t>
         </is>
       </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>2022-08-09</t>
+        </is>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
@@ -4349,6 +5849,11 @@
           <t>http://jud-anexos.digesto.com.br/fdffac80bfd8b15f646ff3bdd5d35e25.html</t>
         </is>
       </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>2023-03-23</t>
+        </is>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="n">
@@ -4362,6 +5867,11 @@
           <t>http://jud-anexos.digesto.com.br/6a3043df0bf815aa7e0435f30440cb90.html</t>
         </is>
       </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>2021-08-31</t>
+        </is>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
@@ -4375,6 +5885,11 @@
           <t>http://jud-anexos.digesto.com.br/1629910174602fcf348b92705bab5d70.html</t>
         </is>
       </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>2019-06-19</t>
+        </is>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="n">
@@ -4388,6 +5903,11 @@
           <t>http://jud-anexos.digesto.com.br/d3c2de4e3bdd7733e70cd082eab2adbe.html</t>
         </is>
       </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>2019-07-31</t>
+        </is>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="n">
@@ -4401,6 +5921,11 @@
           <t>http://jud-anexos.digesto.com.br/0f366aa064cba134ffad21cdbaa1d05b.html</t>
         </is>
       </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>2024-01-09</t>
+        </is>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
@@ -4414,6 +5939,11 @@
           <t>http://jud-anexos.digesto.com.br/1e86208f089453e777a4d6921caaa6c9.pdf</t>
         </is>
       </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>2019-01-21</t>
+        </is>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
@@ -4427,6 +5957,11 @@
           <t>http://jud-anexos.digesto.com.br/b7e39d0557091be3605a459e523174a8.pdf</t>
         </is>
       </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>2021-05-20</t>
+        </is>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
@@ -4440,6 +5975,11 @@
           <t>http://jud-anexos.digesto.com.br/87f558e6991267386391993a230657df.pdf</t>
         </is>
       </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>2021-05-21</t>
+        </is>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
@@ -4453,6 +5993,11 @@
           <t>http://jud-anexos.digesto.com.br/4656af3db95f941aab71836047b03236.pdf</t>
         </is>
       </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>2021-05-21</t>
+        </is>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
@@ -4466,6 +6011,11 @@
           <t>http://jud-anexos.digesto.com.br/c479afb3c201559e5e672bfc5f0335d7.pdf</t>
         </is>
       </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>2021-12-01</t>
+        </is>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
@@ -4479,6 +6029,11 @@
           <t>http://jud-anexos.digesto.com.br/a2cf1c2a5d109c6c5b07fff531e2cb8f.pdf</t>
         </is>
       </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>2021-12-01</t>
+        </is>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
@@ -4492,6 +6047,11 @@
           <t>http://jud-anexos.digesto.com.br/8e8b0cf7cd904bdbf4318daf75b832a4.pdf</t>
         </is>
       </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>2021-12-01</t>
+        </is>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
@@ -4505,6 +6065,11 @@
           <t>http://jud-anexos.digesto.com.br/54b5fdab1e93a4e82cae8a01b295e36c.pdf</t>
         </is>
       </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>2021-12-14</t>
+        </is>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
@@ -4518,6 +6083,11 @@
           <t>http://jud-anexos.digesto.com.br/1f51c12c75ae44954f1e87ee796e0172.pdf</t>
         </is>
       </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>2021-12-16</t>
+        </is>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
@@ -4531,6 +6101,11 @@
           <t>http://jud-anexos.digesto.com.br/e6901245427b2376aeab9f19bfc9998c.pdf</t>
         </is>
       </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>2021-12-16</t>
+        </is>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
@@ -4544,6 +6119,11 @@
           <t>http://jud-anexos.digesto.com.br/461c186be0046c14845e94ca7a18303b.pdf</t>
         </is>
       </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>2024-06-20</t>
+        </is>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
@@ -4557,6 +6137,11 @@
           <t>http://jud-anexos.digesto.com.br/9fbf16a2be29b71a31a8569025a009cf.pdf</t>
         </is>
       </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>2024-07-02</t>
+        </is>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
@@ -4570,6 +6155,11 @@
           <t>http://jud-anexos.digesto.com.br/7e0b3b99de2518a7e58ed7474206311b.pdf</t>
         </is>
       </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>2024-07-02</t>
+        </is>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
@@ -4583,6 +6173,11 @@
           <t>http://jud-anexos.digesto.com.br/ede0777701acdd41c21179cc0bc159e9.pdf</t>
         </is>
       </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>2024-10-15</t>
+        </is>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
@@ -4596,6 +6191,11 @@
           <t>http://jud-anexos.digesto.com.br/2fd2ec7f05f916ba5d41db6642afecba.pdf</t>
         </is>
       </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>2024-10-15</t>
+        </is>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
@@ -4609,6 +6209,11 @@
           <t>http://jud-anexos.digesto.com.br/d29792f44228ea8dbea5d4c4588773df.pdf</t>
         </is>
       </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>2022-09-01</t>
+        </is>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
@@ -4622,6 +6227,11 @@
           <t>http://jud-anexos.digesto.com.br/f6dce6791e83c76c651aa59280fbbe48.pdf</t>
         </is>
       </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>2023-08-18</t>
+        </is>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="n">
@@ -4635,6 +6245,11 @@
           <t>http://jud-anexos.digesto.com.br/efac2275fcb4b5768fbdfb95600ff469.pdf</t>
         </is>
       </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>2021-06-11</t>
+        </is>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="n">
@@ -4648,6 +6263,11 @@
           <t>http://jud-anexos.digesto.com.br/b40d332969a6a6e3da1565f692a3b97f.pdf</t>
         </is>
       </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>2017-11-07</t>
+        </is>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
@@ -4661,6 +6281,11 @@
           <t>http://jud-anexos.digesto.com.br/918ce610fb88deabff8e3128d4f3fc8f.html</t>
         </is>
       </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>2021-10-19</t>
+        </is>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
@@ -4674,6 +6299,11 @@
           <t>http://jud-anexos.digesto.com.br/78e0a7e8929f29ad7144c6dc87cded64.pdf</t>
         </is>
       </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>2019-02-18</t>
+        </is>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
@@ -4687,6 +6317,11 @@
           <t>http://jud-anexos.digesto.com.br/a57439518fb8127b236964cce357313a.pdf</t>
         </is>
       </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>2021-01-20</t>
+        </is>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
@@ -4700,6 +6335,11 @@
           <t>http://jud-anexos.digesto.com.br/f6e75247560187e60f2fe83e2bcdd0c1.pdf</t>
         </is>
       </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>2021-11-08</t>
+        </is>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="n">
@@ -4713,6 +6353,11 @@
           <t>http://jud-anexos.digesto.com.br/606c7db79d938c8923775da581953061.pdf</t>
         </is>
       </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>2021-04-29</t>
+        </is>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="n">
@@ -4726,6 +6371,11 @@
           <t>http://jud-anexos.digesto.com.br/0397b843462ae8b9e0f4d1e4496c591b.pdf</t>
         </is>
       </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>2024-06-17</t>
+        </is>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
@@ -4739,6 +6389,11 @@
           <t>http://jud-anexos.digesto.com.br/8253b946d817f4e5c3dca6ff0755d5bb.pdf</t>
         </is>
       </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>2024-09-13</t>
+        </is>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="n">
@@ -4752,6 +6407,11 @@
           <t>http://jud-anexos.digesto.com.br/37a5cbc58b97d18989d8b98202bc1c99.pdf</t>
         </is>
       </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>2024-11-21</t>
+        </is>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
@@ -4765,6 +6425,11 @@
           <t>http://jud-anexos.digesto.com.br/20b9e19663bbeb7994f1f22ab2aac75f.pdf</t>
         </is>
       </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>2024-10-03</t>
+        </is>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
@@ -4778,6 +6443,11 @@
           <t>http://jud-anexos.digesto.com.br/756f20f73698f48c5f2678b11cb1eeee.pdf</t>
         </is>
       </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>2024-11-26</t>
+        </is>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="n">
@@ -4791,6 +6461,11 @@
           <t>http://jud-anexos.digesto.com.br/d6b42793687b028e24f4d4baa0f20484.pdf</t>
         </is>
       </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>2024-02-29</t>
+        </is>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="n">
@@ -4804,6 +6479,11 @@
           <t>http://jud-anexos.digesto.com.br/d6b42793687b028e24f4d4baa0f20484.pdf</t>
         </is>
       </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>2024-02-29</t>
+        </is>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="n">
@@ -4817,6 +6497,11 @@
           <t>http://jud-anexos.digesto.com.br/f602ece2885b23a2d261faa954612f31.pdf</t>
         </is>
       </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>2023-03-22</t>
+        </is>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
@@ -4830,6 +6515,11 @@
           <t>http://jud-anexos.digesto.com.br/8ad7d0fbbeae8d14a1303530d9bb33be.pdf</t>
         </is>
       </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>2023-05-31</t>
+        </is>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="n">
@@ -4843,6 +6533,11 @@
           <t>http://jud-anexos.digesto.com.br/4f696a2b03b85fcc919fa1bd11e03ad4.pdf</t>
         </is>
       </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>2023-01-31</t>
+        </is>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
@@ -4856,6 +6551,11 @@
           <t>http://jud-anexos.digesto.com.br/da57e9dcc7947457a02763e76c400693.pdf</t>
         </is>
       </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>2022-08-01</t>
+        </is>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
@@ -4869,6 +6569,11 @@
           <t>http://jud-anexos.digesto.com.br/da57e9dcc7947457a02763e76c400693.pdf</t>
         </is>
       </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>2022-08-01</t>
+        </is>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
@@ -4882,6 +6587,11 @@
           <t>http://jud-anexos.digesto.com.br/6006daf474fb687c6f72f2d3eff475e1.pdf</t>
         </is>
       </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>2023-01-18</t>
+        </is>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="n">
@@ -4895,6 +6605,11 @@
           <t>http://jud-anexos.digesto.com.br/9dfc361ae0bd01f226b5ee183cbdc006.pdf</t>
         </is>
       </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>2024-01-12</t>
+        </is>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
@@ -4908,6 +6623,11 @@
           <t>http://jud-anexos.digesto.com.br/9369009ec75dbf5af1f7a8dad32eadcb.pdf</t>
         </is>
       </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>2023-11-16</t>
+        </is>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
@@ -4921,6 +6641,11 @@
           <t>http://jud-anexos.digesto.com.br/dc928111113d8a0d6b25e18a583b9961.pdf</t>
         </is>
       </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>2023-11-20</t>
+        </is>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="n">
@@ -4934,6 +6659,11 @@
           <t>http://jud-anexos.digesto.com.br/a90f3642c268bdf1c89bd998366bad1e.pdf</t>
         </is>
       </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>2024-02-14</t>
+        </is>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="n">
@@ -4947,6 +6677,11 @@
           <t>http://jud-anexos.digesto.com.br/0a1c0238f9d09a10e49cf45745a0cd60.pdf</t>
         </is>
       </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>2015-09-29</t>
+        </is>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="n">
@@ -4960,6 +6695,11 @@
           <t>http://jud-anexos.digesto.com.br/a81435ba2bec58eeb8401530111679aa.pdf</t>
         </is>
       </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>2025-01-02</t>
+        </is>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="n">
@@ -4973,6 +6713,11 @@
           <t>http://jud-anexos.digesto.com.br/76754de63b532d7a1322ddc783dfcdf0.pdf</t>
         </is>
       </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>2022-09-19</t>
+        </is>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
@@ -4986,6 +6731,11 @@
           <t>http://jud-anexos.digesto.com.br/569fa73471de9d038491b184fa1499da.pdf</t>
         </is>
       </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>2018-10-19</t>
+        </is>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
@@ -4999,6 +6749,11 @@
           <t>http://jud-anexos.digesto.com.br/20a7431e74b8f6bccea6a17a03eac0ef.pdf</t>
         </is>
       </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>2016-11-18</t>
+        </is>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="n">
@@ -5012,6 +6767,11 @@
           <t>http://jud-anexos.digesto.com.br/e7afe2da7882ff4fd1947dfb0a430225.pdf</t>
         </is>
       </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>2015-05-18</t>
+        </is>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="n">
@@ -5025,6 +6785,11 @@
           <t>http://jud-anexos.digesto.com.br/880101b63ac7dbfbbdf23c1e46be65c1.pdf</t>
         </is>
       </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>2020-09-21</t>
+        </is>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="n">
@@ -5038,6 +6803,11 @@
           <t>http://jud-anexos.digesto.com.br/4641269f43803d27f00d5160585f4e6f.pdf</t>
         </is>
       </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>2021-04-05</t>
+        </is>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="n">
@@ -5051,6 +6821,11 @@
           <t>http://jud-anexos.digesto.com.br/7e4bacb67aed6e5181e01b48fe87c3b7.pdf</t>
         </is>
       </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>2021-05-25</t>
+        </is>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="n">
@@ -5064,6 +6839,11 @@
           <t>http://jud-anexos.digesto.com.br/6f3ed4a7da560650e4718304e24b3974.pdf</t>
         </is>
       </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>2020-11-26</t>
+        </is>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="n">
@@ -5077,6 +6857,11 @@
           <t>http://jud-anexos.digesto.com.br/a036ae039c24b84949a6402d160caa69.pdf</t>
         </is>
       </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>2021-01-12</t>
+        </is>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="n">
@@ -5090,6 +6875,11 @@
           <t>http://jud-anexos.digesto.com.br/a036ae039c24b84949a6402d160caa69.pdf</t>
         </is>
       </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>2021-01-12</t>
+        </is>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="n">
@@ -5103,6 +6893,11 @@
           <t>http://jud-anexos.digesto.com.br/7c08ee8afc968d1a95fff203abf6ac27.pdf</t>
         </is>
       </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>2023-08-31</t>
+        </is>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="n">
@@ -5116,6 +6911,11 @@
           <t>http://jud-anexos.digesto.com.br/8608a63b4b18e4c8661ad3f940a8dd06.pdf</t>
         </is>
       </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>2019-02-18</t>
+        </is>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="n">
@@ -5129,6 +6929,11 @@
           <t>http://jud-anexos.digesto.com.br/990b5e04f51f93499d9e5e6f68959963.pdf</t>
         </is>
       </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>2017-10-19</t>
+        </is>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="n">
@@ -5142,6 +6947,11 @@
           <t>http://jud-anexos.digesto.com.br/e2b845bb26f04e4a73875c1593b64a51.pdf</t>
         </is>
       </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>2020-09-10</t>
+        </is>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="n">
@@ -5155,6 +6965,11 @@
           <t>http://jud-anexos.digesto.com.br/e2b845bb26f04e4a73875c1593b64a51.pdf</t>
         </is>
       </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>2020-09-11</t>
+        </is>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="n">
@@ -5168,6 +6983,11 @@
           <t>http://jud-anexos.digesto.com.br/c3d0e5109b664160a76a255a5b0e23e3.pdf</t>
         </is>
       </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>2013-05-29</t>
+        </is>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="n">
@@ -5181,6 +7001,11 @@
           <t>http://jud-anexos.digesto.com.br/46924d57688a75d0fcec3cb2e85bb4aa.pdf</t>
         </is>
       </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>2016-11-01</t>
+        </is>
+      </c>
     </row>
     <row r="366">
       <c r="A366" t="n">
@@ -5194,6 +7019,11 @@
           <t>http://jud-anexos.digesto.com.br/f1524592401e6b27cda87089ecf3de14.pdf</t>
         </is>
       </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>2021-12-15</t>
+        </is>
+      </c>
     </row>
     <row r="367">
       <c r="A367" t="n">
@@ -5207,6 +7037,11 @@
           <t>http://jud-anexos.digesto.com.br/714958f05a7b734096f7f4df3aeb3437.pdf</t>
         </is>
       </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>2020-03-12</t>
+        </is>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="n">
@@ -5220,6 +7055,11 @@
           <t>http://jud-anexos.digesto.com.br/12b8586023ed46bc17f3a6ce223435cc.pdf</t>
         </is>
       </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>2020-05-13</t>
+        </is>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="n">
@@ -5233,6 +7073,11 @@
           <t>http://jud-anexos.digesto.com.br/96f5d5479af6ae74a82fda8a616421c1.pdf</t>
         </is>
       </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>2021-04-27</t>
+        </is>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="n">
@@ -5246,6 +7091,11 @@
           <t>http://jud-anexos.digesto.com.br/b1893d4135d19920f387e3395c9c0763.pdf</t>
         </is>
       </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>2023-01-17</t>
+        </is>
+      </c>
     </row>
     <row r="371">
       <c r="A371" t="n">
@@ -5259,6 +7109,11 @@
           <t>http://jud-anexos.digesto.com.br/f4e7744f1ff466f9dc4b5dd3e2a19ec8.pdf</t>
         </is>
       </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>2020-03-28</t>
+        </is>
+      </c>
     </row>
     <row r="372">
       <c r="A372" t="n">
@@ -5272,6 +7127,11 @@
           <t>http://jud-anexos.digesto.com.br/7293071fe37ba77d19e67cf4fddc6f17.pdf</t>
         </is>
       </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>2018-10-21</t>
+        </is>
+      </c>
     </row>
     <row r="373">
       <c r="A373" t="n">
@@ -5285,6 +7145,11 @@
           <t>http://jud-anexos.digesto.com.br/05f7ea3480cba64e425e19976dd40fe8.pdf</t>
         </is>
       </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>2024-10-29</t>
+        </is>
+      </c>
     </row>
     <row r="374">
       <c r="A374" t="n">
@@ -5298,6 +7163,11 @@
           <t>http://jud-anexos.digesto.com.br/70aeaf7e20395d8aa0642ff7d5aada53.pdf</t>
         </is>
       </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>2016-08-12</t>
+        </is>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="n">
@@ -5311,6 +7181,11 @@
           <t>http://jud-anexos.digesto.com.br/f11ee0ac37884a0055577b1b65c48dbe.pdf</t>
         </is>
       </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>2022-05-09</t>
+        </is>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="n">
@@ -5324,6 +7199,11 @@
           <t>http://jud-anexos.digesto.com.br/a85dc0619493fbcfe1d4cb1d3a543a47.pdf</t>
         </is>
       </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>2021-11-05</t>
+        </is>
+      </c>
     </row>
     <row r="377">
       <c r="A377" t="n">
@@ -5337,6 +7217,11 @@
           <t>http://jud-anexos.digesto.com.br/5e6ace718d8c1a2eeeea72fb51129708.pdf</t>
         </is>
       </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>2022-03-17</t>
+        </is>
+      </c>
     </row>
     <row r="378">
       <c r="A378" t="n">
@@ -5350,6 +7235,11 @@
           <t>http://jud-anexos.digesto.com.br/ceed0280ba8384aa38f16005e21a4a7a.pdf</t>
         </is>
       </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>2021-02-05</t>
+        </is>
+      </c>
     </row>
     <row r="379">
       <c r="A379" t="n">
@@ -5363,6 +7253,11 @@
           <t>http://jud-anexos.digesto.com.br/53d4321ebd1abe839d9216b6a2f875c4.pdf</t>
         </is>
       </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>2021-04-26</t>
+        </is>
+      </c>
     </row>
     <row r="380">
       <c r="A380" t="n">
@@ -5376,6 +7271,11 @@
           <t>http://jud-anexos.digesto.com.br/b8db09ceabfe54bef91a64ab36100011.pdf</t>
         </is>
       </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>2020-11-16</t>
+        </is>
+      </c>
     </row>
     <row r="381">
       <c r="A381" t="n">
@@ -5389,6 +7289,11 @@
           <t>http://jud-anexos.digesto.com.br/f319402c4d9b7f1bc09a5d5891d9f717.pdf</t>
         </is>
       </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>2022-08-25</t>
+        </is>
+      </c>
     </row>
     <row r="382">
       <c r="A382" t="n">
@@ -5402,6 +7307,11 @@
           <t>http://jud-anexos.digesto.com.br/5208e82aa91f775e966578f21d640a81.pdf</t>
         </is>
       </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>2020-06-23</t>
+        </is>
+      </c>
     </row>
     <row r="383">
       <c r="A383" t="n">
@@ -5415,6 +7325,11 @@
           <t>http://jud-anexos.digesto.com.br/b090125f6e001545ed6c64c270b4128e.pdf</t>
         </is>
       </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>2022-01-19</t>
+        </is>
+      </c>
     </row>
     <row r="384">
       <c r="A384" t="n">
@@ -5428,6 +7343,11 @@
           <t>http://jud-anexos.digesto.com.br/b090125f6e001545ed6c64c270b4128e.pdf</t>
         </is>
       </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>2022-01-19</t>
+        </is>
+      </c>
     </row>
     <row r="385">
       <c r="A385" t="n">
@@ -5441,6 +7361,11 @@
           <t>http://jud-anexos.digesto.com.br/c439b4be278ace182e79d69d11b012a2.pdf</t>
         </is>
       </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>2015-02-18</t>
+        </is>
+      </c>
     </row>
     <row r="386">
       <c r="A386" t="n">
@@ -5454,6 +7379,11 @@
           <t>http://jud-anexos.digesto.com.br/df6e3e8da998772654df2b00f7d86579.pdf</t>
         </is>
       </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
     </row>
     <row r="387">
       <c r="A387" t="n">
@@ -5467,6 +7397,11 @@
           <t>http://jud-anexos.digesto.com.br/f1bb256d76c0d25b7980ca251ae7c293.pdf</t>
         </is>
       </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>2024-08-23</t>
+        </is>
+      </c>
     </row>
     <row r="388">
       <c r="A388" t="n">
@@ -5480,6 +7415,11 @@
           <t>http://jud-anexos.digesto.com.br/218cc27fba45381e6b369e994f508031.pdf</t>
         </is>
       </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
     </row>
     <row r="389">
       <c r="A389" t="n">
@@ -5493,6 +7433,11 @@
           <t>http://jud-anexos.digesto.com.br/8ab01c9d05320b2f96c5536634efa4f8.html</t>
         </is>
       </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>2024-10-01</t>
+        </is>
+      </c>
     </row>
     <row r="390">
       <c r="A390" t="n">
@@ -5506,6 +7451,11 @@
           <t>http://jud-anexos.digesto.com.br/e55b90bdcd194e97c68f4c8754c17646.pdf</t>
         </is>
       </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>2022-05-01</t>
+        </is>
+      </c>
     </row>
     <row r="391">
       <c r="A391" t="n">
@@ -5519,6 +7469,11 @@
           <t>http://jud-anexos.digesto.com.br/e3f977a11a4d1137ea8dfe077a9a5c17.html</t>
         </is>
       </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>2022-05-01</t>
+        </is>
+      </c>
     </row>
     <row r="392">
       <c r="A392" t="n">
@@ -5532,6 +7487,11 @@
           <t>http://jud-anexos.digesto.com.br/4c97bd2fdb0615140fa5c0b4432da05e.html</t>
         </is>
       </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>2022-05-17</t>
+        </is>
+      </c>
     </row>
     <row r="393">
       <c r="A393" t="n">
@@ -5543,6 +7503,11 @@
       <c r="C393" t="inlineStr">
         <is>
           <t>http://jud-anexos.digesto.com.br/dce333e4d851f163a94f62103aef5f44.pdf</t>
+        </is>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>2022-05-17</t>
         </is>
       </c>
     </row>

</xml_diff>